<commit_message>
Fixed Q4 demo spreadsheet
</commit_message>
<xml_diff>
--- a/tests/fixtures/bundles/Smart-seq2/Q4DemoSS2Metadata.xlsx
+++ b/tests/fixtures/bundles/Smart-seq2/Q4DemoSS2Metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19440" yWindow="10700" windowWidth="25600" windowHeight="13860" activeTab="6"/>
+    <workbookView xWindow="2440" yWindow="3060" windowWidth="25600" windowHeight="13860" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="71">
   <si>
     <t>id</t>
   </si>
@@ -247,13 +247,10 @@
     <t>seq.lanes.run</t>
   </si>
   <si>
-    <t>Q3_DEMO-sample_SAMN02797092_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>Q3_DEMO-sample_SAMN02797092_R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>seq.insdc_experiment</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>single cell sequencing</t>
   </si>
 </sst>
 </file>
@@ -389,7 +386,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -405,9 +402,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="30">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -973,20 +967,19 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.33203125" customWidth="1"/>
-    <col min="7" max="7" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -1005,11 +998,8 @@
       <c r="F1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1017,7 +1007,7 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
         <v>36</v>
@@ -1028,11 +1018,8 @@
       <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -1040,7 +1027,7 @@
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
         <v>36</v>
@@ -1050,9 +1037,6 @@
       </c>
       <c r="F3" t="s">
         <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1075,12 +1059,12 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>42</v>
@@ -1099,7 +1083,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:B2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1109,12 +1093,12 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>42</v>
@@ -1254,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1265,20 +1249,26 @@
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1290,7 +1280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Change metadata spreadsheet, File tab file format heading to 'file_format'
</commit_message>
<xml_diff>
--- a/tests/fixtures/bundles/Smart-seq2/Q4DemoSS2Metadata.xlsx
+++ b/tests/fixtures/bundles/Smart-seq2/Q4DemoSS2Metadata.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/Science/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sampierson/Development/HCA/dcp/tests/fixtures/bundles/Smart-seq2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="3060" windowWidth="25600" windowHeight="13860" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="-33520" yWindow="12380" windowWidth="33520" windowHeight="20540" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -61,9 +61,6 @@
     <t>sample_id</t>
   </si>
   <si>
-    <t>format</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>single cell sequencing</t>
+  </si>
+  <si>
+    <t>file_format</t>
   </si>
 </sst>
 </file>
@@ -745,18 +745,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -764,7 +764,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -809,16 +809,16 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>5</v>
@@ -830,7 +830,7 @@
         <v>3</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -838,34 +838,34 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -937,27 +937,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="210" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -981,62 +981,62 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>67</v>
-      </c>
-      <c r="F1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
         <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1059,15 +1059,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1093,15 +1093,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1136,27 +1136,27 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>9606</v>
@@ -1187,7 +1187,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -1196,39 +1196,39 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" t="s">
-        <v>49</v>
-      </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
       </c>
       <c r="F2">
         <v>9606</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1251,24 +1251,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1296,17 +1296,17 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2"/>
       <c r="F2" s="1"/>
@@ -1353,28 +1353,28 @@
   <sheetData>
     <row r="1" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
@@ -1400,13 +1400,13 @@
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="2"/>
       <c r="H2" s="1"/>
@@ -1461,16 +1461,16 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
@@ -1485,16 +1485,16 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>

</xml_diff>